<commit_message>
Fixed a stupid bug with droplets walking. Good, but it through off all of my calibration values.
</commit_message>
<xml_diff>
--- a/MotorCalibrationValues/OldDroplets.xlsx
+++ b/MotorCalibrationValues/OldDroplets.xlsx
@@ -75,10 +75,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -384,7 +384,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,11 +402,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3">
@@ -420,7 +420,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4">
@@ -433,86 +433,41 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>250</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="1"/>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>-1</v>
-      </c>
-      <c r="D5">
-        <v>136</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="1"/>
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6">
-        <v>-100</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>-1</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="1"/>
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>-120</v>
-      </c>
-      <c r="E7">
-        <v>-1</v>
-      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="1"/>
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8">
-        <v>100</v>
-      </c>
-      <c r="D8">
-        <v>-1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="1"/>
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>310</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="1"/>
       <c r="B10">
         <v>6</v>
       </c>
@@ -520,22 +475,22 @@
         <v>-1</v>
       </c>
       <c r="D10">
-        <v>-10</v>
+        <v>-5</v>
       </c>
       <c r="E10">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="1"/>
       <c r="B11">
         <v>7</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="D11">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="E11">
         <v>-1</v>
@@ -550,11 +505,11 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14">
@@ -568,7 +523,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B15">
@@ -576,37 +531,37 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="1"/>
       <c r="B16">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="1"/>
       <c r="B17">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="1"/>
       <c r="B18">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="1"/>
       <c r="B19">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="1"/>
       <c r="B20">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="1"/>
       <c r="B21">
         <v>6</v>
       </c>
@@ -621,7 +576,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="1"/>
       <c r="B22">
         <v>7</v>
       </c>
@@ -644,11 +599,11 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="C24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25">
@@ -662,7 +617,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B26">
@@ -679,7 +634,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="A27" s="1"/>
       <c r="B27">
         <v>1</v>
       </c>
@@ -694,13 +649,13 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="A28" s="1"/>
       <c r="B28">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+      <c r="A29" s="1"/>
       <c r="B29">
         <v>3</v>
       </c>
@@ -715,19 +670,19 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
+      <c r="A30" s="1"/>
       <c r="B30">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
+      <c r="A31" s="1"/>
       <c r="B31">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
+      <c r="A32" s="1"/>
       <c r="B32">
         <v>6</v>
       </c>
@@ -742,7 +697,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
+      <c r="A33" s="1"/>
       <c r="B33">
         <v>7</v>
       </c>

</xml_diff>